<commit_message>
Fix Default Code In Import Excel Of Suppliers, Services, Products, Medicines
</commit_message>
<xml_diff>
--- a/TMTDentalAPI/ClientApp/src/assets/files/MauFileDichVu.xlsx
+++ b/TMTDentalAPI/ClientApp/src/assets/files/MauFileDichVu.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGA\Documents\Projects\TDental\TMTDentalAPI\ClientApp\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\TDental\TMTDentalAPI\ClientApp\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
     <author>GIGA</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Giá bán</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Nhóm dịch vụ</t>
-  </si>
-  <si>
-    <t>Mã dịch vụ</t>
   </si>
   <si>
     <t>Công đoạn 1;Công đoạn 2;Công đoạn 3</t>
@@ -415,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,13 +423,12 @@
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -442,22 +438,19 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -465,13 +458,13 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="D2" s="3">
         <v>100000</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>